<commit_message>
Completion of sandbox 2. Code tidied up a bit more with the update methods separated. Balloon has a lot more variables and an intersects method and two states, alive or dead. Debug screen now shows the amount of spawns total. Balloons can be popped with a single tap, no multi-touch.
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,9 +1010,21 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
       <c r="G3" s="3"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="3"/>
+      <c r="L3" s="18"/>
       <c r="M3" s="18"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added a sound file to the balloon objects to play when they are popped. Controls doesn't assign a balloon object anymore, it just calls pop on the last one in the list. Increased the speed for the balloons to spawn to one every 2.5s and the memory pool up to 7. Updated the plan to reflect the changes made for sandbox 3 and the animation feature has been flagged to be done.
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,7 +992,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
@@ -1025,6 +1025,35 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed the explosion sound to something more subtle. Added the explosion animation effect and is centred to the popping balloon. Balloon code needs tidying up.
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Game Section</t>
   </si>
@@ -148,13 +148,25 @@
   </si>
   <si>
     <t>Controls</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Tentative</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +211,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -223,7 +244,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -347,6 +368,21 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -358,13 +394,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -378,8 +413,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -389,6 +422,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -712,207 +754,207 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="8"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="9"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="9"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="17"/>
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="9"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="9"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="9"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="9"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="9"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="17"/>
+      <c r="B11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="9"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="9"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="9"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="17"/>
+      <c r="B14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="9"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="9"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="9"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="9" t="s">
+      <c r="A17" s="17"/>
+      <c r="B17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="9"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="9"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="9"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="9" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="9"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="10" t="s">
+      <c r="A21" s="18"/>
+      <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="10"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -927,14 +969,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -947,116 +990,149 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="21"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="22"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="23"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B6" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D6" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F6" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G6" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H6" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I6" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J6" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K6" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L6" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M6" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="24">
         <v>3</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Sandbox 3 final. Tidied up the animation code to allow for animations of one frame, balloon code now uses two animations instead of drawing a texture, everything can now be animated easily. When app deactivated the game will exit completely  instead, previously when reactivated the spawn counter wouldn't have changed but everything else would've reset. Plan updated to include sandbox 4. New textures for the app thumb and tile added. Timer renamed to SpawnTimer.
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>Game Section</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Snowflake</t>
   </si>
 </sst>
 </file>
@@ -394,7 +397,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -413,6 +416,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -422,15 +434,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -771,7 +775,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -782,7 +786,7 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
@@ -791,7 +795,7 @@
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
@@ -800,7 +804,7 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
@@ -809,7 +813,7 @@
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
@@ -818,7 +822,7 @@
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="12" t="s">
         <v>11</v>
       </c>
@@ -827,7 +831,7 @@
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -838,7 +842,7 @@
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="9" t="s">
         <v>14</v>
       </c>
@@ -847,7 +851,7 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="24" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -858,7 +862,7 @@
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="8" t="s">
         <v>17</v>
       </c>
@@ -867,7 +871,7 @@
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="8" t="s">
         <v>18</v>
       </c>
@@ -876,7 +880,7 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="8" t="s">
         <v>19</v>
       </c>
@@ -885,7 +889,7 @@
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="8" t="s">
         <v>20</v>
       </c>
@@ -894,7 +898,7 @@
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="8" t="s">
         <v>21</v>
       </c>
@@ -903,7 +907,7 @@
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="8" t="s">
         <v>22</v>
       </c>
@@ -912,7 +916,7 @@
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="8" t="s">
         <v>23</v>
       </c>
@@ -921,7 +925,7 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
@@ -930,7 +934,7 @@
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="8" t="s">
         <v>25</v>
       </c>
@@ -939,7 +943,7 @@
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="8" t="s">
         <v>26</v>
       </c>
@@ -948,7 +952,7 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
@@ -969,10 +973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,147 +991,155 @@
     <col min="9" max="9" width="8" customWidth="1"/>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="21"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="B2" s="18"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="22"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="B3" s="19"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="23"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="B4" s="20"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="J6" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="25" t="s">
+      <c r="K6" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="L6" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="25" t="s">
+      <c r="M6" s="22" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="24">
+      <c r="N6" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
         <v>1</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="24">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
         <v>2</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="24">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="20"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
         <v>3</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="24">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="20"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
         <v>4</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sandbox 4. Added a new variable spawn timer. Added all three balloons to timers. Green on a mono timer, the other two on variable timers. Added score and suns mood although only score updates, mood isn't affected. Debug information in the bottom left hand corner. All three balloons have their own move animation. New text file for displaying score and mood.
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>Game Section</t>
   </si>
@@ -400,12 +400,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -429,6 +428,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -437,9 +439,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -750,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -764,19 +763,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -784,193 +783,193 @@
       <c r="A2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="7"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="8"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="8"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26"/>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="8"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="26"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="8"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="8"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="8"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="8"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="8"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="8"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="8"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="8"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="26"/>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="9"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -987,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,146 +1006,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="18"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="19"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="L6" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="22" t="s">
+      <c r="M6" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N6" s="23" t="s">
+      <c r="N6" s="22" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="A7" s="20">
         <v>1</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="20">
         <v>2</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="20"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="19"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+      <c r="A9" s="20">
         <v>3</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="20"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="20">
         <v>4</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="18"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="20"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="19"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="20">
+        <v>5</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="19"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -1162,59 +1176,107 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="19"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B6" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E6" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F6" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G6" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H6" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I6" s="21" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="J6" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
         <v>2</v>
       </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sandbox 5 start. Added game state and the ability to change from playing to game over.
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Game Section</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Game State</t>
   </si>
 </sst>
 </file>
@@ -984,10 +987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:N11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,32 +1006,33 @@
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="17"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="18"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B4" s="19"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>28</v>
       </c>
@@ -1071,8 +1075,11 @@
       <c r="N6" s="22" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>1</v>
       </c>
@@ -1089,8 +1096,9 @@
       <c r="L7" s="19"/>
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="19"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>2</v>
       </c>
@@ -1107,8 +1115,9 @@
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
       <c r="N8" s="19"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="19"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>3</v>
       </c>
@@ -1125,8 +1134,9 @@
       <c r="L9" s="18"/>
       <c r="M9" s="18"/>
       <c r="N9" s="19"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="19"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>4</v>
       </c>
@@ -1143,8 +1153,9 @@
       <c r="L10" s="18"/>
       <c r="M10" s="18"/>
       <c r="N10" s="19"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="19"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>5</v>
       </c>
@@ -1161,11 +1172,12 @@
       <c r="L11" s="18"/>
       <c r="M11" s="18"/>
       <c r="N11" s="19"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="18"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sandbox 5. Added a simple power up mechanic. Cleaned up some variables in the balloon. All collisions are now done in a new collisions class. Only the freeze power up is available and has no effects, borrows the pop sound and animation.
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -990,7 +990,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1171,7 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
       <c r="M11" s="18"/>
-      <c r="N11" s="19"/>
+      <c r="N11" s="18"/>
       <c r="O11" s="18"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Sandbox 5 final. Optimised the player input update to use loops and go backwards and exit on the first power up or balloon that has been hit. Tidied up the balloon and power up class. Fixed the sound effect problem by playing the sound sound effect once as it is loaded, to prevent the stuttering of popping the first balloon.
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -403,11 +403,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -766,213 +763,213 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="7"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="7"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="10" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="7"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="11" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="7"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="24"/>
+      <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="7"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="24"/>
+      <c r="B13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="7"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="24"/>
+      <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="7"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="7"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="24"/>
+      <c r="B16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="7"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="24"/>
+      <c r="B17" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="7"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="24"/>
+      <c r="B18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="24"/>
+      <c r="B19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="24"/>
+      <c r="B20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="25"/>
+      <c r="B21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="8"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -990,7 +987,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,175 +1007,207 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="18"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="21" t="s">
+      <c r="L6" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="21" t="s">
+      <c r="M6" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="N6" s="22" t="s">
+      <c r="N6" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="O6" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="A7" s="19">
         <v>1</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+      <c r="A8" s="19">
         <v>2</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
+      <c r="A9" s="19">
         <v>3</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
+      <c r="A10" s="19">
         <v>4</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
+      <c r="A11" s="19">
         <v>5</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="19">
+        <v>6</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="19">
+        <v>7</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1208,87 +1237,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="16"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="18"/>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="18"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="20" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="A7" s="19">
         <v>1</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+      <c r="A8" s="19">
         <v>2</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sandbox 6. The freeze ability now freezes all balloons on screen but not those that spawn after it has been applied. Spotted a scaling problem with the pop animation and its positioning. It may need to be resized and scaled before importing. Then the balloon would need to have a global scale to apply to all animations to have scaled pops for each size of balloon. Plan updated with the notion to put everything into a manager.
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
   <si>
     <t>Game Section</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Sun</t>
+  </si>
+  <si>
+    <t>Character Managers</t>
   </si>
 </sst>
 </file>
@@ -443,6 +446,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -452,8 +457,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -763,7 +766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -794,7 +797,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -805,7 +808,7 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
@@ -814,7 +817,7 @@
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
@@ -823,7 +826,7 @@
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
@@ -832,7 +835,7 @@
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
@@ -841,7 +844,7 @@
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
@@ -850,7 +853,7 @@
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="26" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -861,7 +864,7 @@
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
@@ -870,7 +873,7 @@
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="27" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -883,7 +886,7 @@
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
@@ -894,7 +897,7 @@
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
+      <c r="A12" s="27"/>
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
@@ -905,7 +908,7 @@
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="6" t="s">
         <v>19</v>
       </c>
@@ -916,7 +919,7 @@
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
@@ -927,7 +930,7 @@
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="6" t="s">
         <v>21</v>
       </c>
@@ -936,7 +939,7 @@
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="6" t="s">
         <v>22</v>
       </c>
@@ -945,7 +948,7 @@
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="6" t="s">
         <v>55</v>
       </c>
@@ -954,7 +957,7 @@
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="6" t="s">
         <v>23</v>
       </c>
@@ -963,7 +966,7 @@
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="6" t="s">
         <v>24</v>
       </c>
@@ -972,7 +975,7 @@
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="27"/>
       <c r="B20" s="6" t="s">
         <v>25</v>
       </c>
@@ -981,7 +984,7 @@
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="6" t="s">
         <v>26</v>
       </c>
@@ -992,7 +995,7 @@
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="6" t="s">
         <v>27</v>
       </c>
@@ -1001,28 +1004,28 @@
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="21"/>
-      <c r="D23" s="27"/>
+      <c r="D23" s="24"/>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="21"/>
-      <c r="D24" s="27"/>
+      <c r="D24" s="24"/>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="7"/>
       <c r="C25" s="23"/>
-      <c r="D25" s="28"/>
+      <c r="D25" s="25"/>
       <c r="E25" s="7"/>
     </row>
   </sheetData>
@@ -1038,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,32 +1062,33 @@
     <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="15"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="16"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B4" s="17"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>28</v>
       </c>
@@ -1136,8 +1140,11 @@
       <c r="Q6" s="20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>1</v>
       </c>
@@ -1157,8 +1164,9 @@
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="17"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="17"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
         <v>2</v>
       </c>
@@ -1178,8 +1186,9 @@
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="17"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" s="17"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>3</v>
       </c>
@@ -1199,8 +1208,9 @@
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="17"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9" s="17"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="18">
         <v>4</v>
       </c>
@@ -1220,8 +1230,9 @@
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" s="17"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>5</v>
       </c>
@@ -1241,19 +1252,20 @@
       <c r="O11" s="16"/>
       <c r="P11" s="16"/>
       <c r="Q11" s="17"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" s="17"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="18">
         <v>6</v>
       </c>
       <c r="B12" s="16"/>
       <c r="C12" s="15"/>
       <c r="D12" s="16"/>
-      <c r="E12" s="14"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="16"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="14"/>
@@ -1261,9 +1273,10 @@
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
       <c r="P12" s="16"/>
-      <c r="Q12" s="14"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q12" s="16"/>
+      <c r="R12" s="17"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>7</v>
       </c>
@@ -1283,6 +1296,7 @@
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sandbox 6 final. Plan updated. Green balloon has green move animation.
Signed-off-by: Joshua Hirst <hirst.joshua@me.com>
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>Game Section</t>
   </si>
@@ -132,18 +132,12 @@
     <t>Splash View</t>
   </si>
   <si>
-    <t>H&amp;S View</t>
-  </si>
-  <si>
     <t>Main Menu</t>
   </si>
   <si>
     <t>Score Anim.</t>
   </si>
   <si>
-    <t>Code Optimised</t>
-  </si>
-  <si>
     <t>Collisions</t>
   </si>
   <si>
@@ -186,7 +180,19 @@
     <t>Sun</t>
   </si>
   <si>
-    <t>Character Managers</t>
+    <t>Optimised</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Shotgun</t>
+  </si>
+  <si>
+    <t>Balloon Manager</t>
   </si>
 </sst>
 </file>
@@ -232,15 +238,14 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="22"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +267,12 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -413,7 +424,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -427,7 +438,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1"/>
@@ -448,6 +458,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -455,6 +470,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -797,235 +815,235 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="21"/>
       <c r="D2" s="11"/>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="12"/>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="12"/>
       <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="12"/>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="12"/>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="12"/>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="28" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="12"/>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="12"/>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="29" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>49</v>
+      <c r="C10" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>49</v>
+      <c r="C11" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>49</v>
+      <c r="C12" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="21" t="s">
-        <v>49</v>
+      <c r="C13" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="21" t="s">
-        <v>49</v>
+      <c r="C14" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="12"/>
       <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="21"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="12"/>
       <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="21"/>
+        <v>53</v>
+      </c>
+      <c r="C17" s="20"/>
       <c r="D17" s="12"/>
       <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="21"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="12"/>
       <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="12"/>
       <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="21"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="12"/>
       <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="21" t="s">
-        <v>49</v>
+      <c r="C21" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="21"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="12"/>
       <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="24"/>
+        <v>51</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="24"/>
+        <v>52</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="7"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="25"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="24"/>
       <c r="E25" s="7"/>
     </row>
   </sheetData>
@@ -1041,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,244 +1077,254 @@
     <col min="9" max="9" width="10.28515625" customWidth="1"/>
     <col min="10" max="10" width="8" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="14"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="B3" s="15"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="15"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="B4" s="16"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="16"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="17"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="O6" s="20" t="s">
+      <c r="P6" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="P6" s="19" t="s">
+      <c r="Q6" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="Q6" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="R6" s="20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="R6" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
         <v>1</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
         <v>2</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="B8" s="15"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
         <v>3</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
+      <c r="B9" s="15"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
         <v>4</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+      <c r="B10" s="15"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
         <v>5</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="B11" s="15"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
         <v>6</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="17"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="B12" s="15"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
         <v>7</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1306,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,98 +1345,136 @@
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="E2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="E3" s="13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="F3" s="15"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="E4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="15"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="16"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="17"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="F4" s="16"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="19" t="s">
+      <c r="H6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="I6" s="18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="J6" s="25"/>
+      <c r="K6" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
         <v>1</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="16"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
         <v>2</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="13"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C4"/>
+    <mergeCell ref="J1:L4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sandbox 7. Player and weapon classes under construction, not used yet. Game now resets and has a score but, recreates the managers and player, need a reset method.
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
-    <sheet name="Balloon Sandbox" sheetId="2" r:id="rId2"/>
+    <sheet name="Game Sandbox" sheetId="2" r:id="rId2"/>
     <sheet name="Menu Sandbox" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t>Game Section</t>
   </si>
@@ -189,10 +189,13 @@
     <t>Maintenance</t>
   </si>
   <si>
-    <t>Shotgun</t>
-  </si>
-  <si>
-    <t>Balloon Manager</t>
+    <t>Character Managers</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Weapon</t>
   </si>
 </sst>
 </file>
@@ -1059,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,30 +1086,30 @@
     <col min="18" max="18" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B3" s="15"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B4" s="16"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>28</v>
       </c>
@@ -1159,13 +1162,16 @@
         <v>50</v>
       </c>
       <c r="R6" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="S6" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="S6" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T6" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>1</v>
       </c>
@@ -1187,8 +1193,9 @@
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
       <c r="S7" s="16"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T7" s="16"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
         <v>2</v>
       </c>
@@ -1210,8 +1217,9 @@
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
       <c r="S8" s="16"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T8" s="16"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>3</v>
       </c>
@@ -1233,8 +1241,9 @@
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
       <c r="S9" s="16"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T9" s="16"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>4</v>
       </c>
@@ -1256,8 +1265,9 @@
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T10" s="16"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>5</v>
       </c>
@@ -1279,8 +1289,9 @@
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
       <c r="S11" s="16"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T11" s="16"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>6</v>
       </c>
@@ -1302,29 +1313,55 @@
       <c r="Q12" s="15"/>
       <c r="R12" s="16"/>
       <c r="S12" s="16"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T12" s="16"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>7</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>8</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>